<commit_message>
Gjort om testcases till svenska och gjort så den passar utmärkt i word
</commit_message>
<xml_diff>
--- a/Administrativa Filer/TestCases.xlsx
+++ b/Administrativa Filer/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D865B4E-88FA-49E7-B55A-DFFFE1ADA96B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C145CC-AA45-47A5-9EBA-5AD96AE2C6F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1500" windowWidth="29040" windowHeight="15840" xr2:uid="{DFD00660-DC2C-47B0-B7C6-F54E6FD6251E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DFD00660-DC2C-47B0-B7C6-F54E6FD6251E}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,91 +31,136 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
-  <si>
-    <t>Test Case</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>Launch site</t>
-  </si>
-  <si>
-    <t>Go to http://90.224.160.35/</t>
-  </si>
-  <si>
-    <t>Front page appears</t>
-  </si>
-  <si>
-    <t>Browse products</t>
-  </si>
-  <si>
-    <t>The requested product page should appear.</t>
-  </si>
-  <si>
-    <t>The product page appears</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create a user </t>
-  </si>
-  <si>
-    <t>Press the user tab. Then fill out the regristation form.</t>
-  </si>
-  <si>
     <t>Null</t>
   </si>
   <si>
-    <t>Not implemented.</t>
-  </si>
-  <si>
-    <t>Place an order using the shopping cart</t>
-  </si>
-  <si>
-    <t>Go to the product page and press buy. After you're satisified, go to the shopping cart and press order.</t>
-  </si>
-  <si>
-    <t>Go to the product page and scroll all the way down, then leave a comment/grade while logged in.</t>
-  </si>
-  <si>
-    <t>Leave a comment and give it a grade</t>
-  </si>
-  <si>
-    <t>Press the navigation bar, choose a product category and then an option.</t>
-  </si>
-  <si>
-    <t>The front page should appear.</t>
-  </si>
-  <si>
-    <t>A user with your credentials should now exist.</t>
-  </si>
-  <si>
-    <t>A comment/grade should be made and displayed.</t>
-  </si>
-  <si>
-    <t>A order should be dispatched and the shoppingcart should be emptied.</t>
-  </si>
-  <si>
-    <t>Pass</t>
+    <t>Förväntat resultat</t>
+  </si>
+  <si>
+    <t>Resultat</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Not</t>
+  </si>
+  <si>
+    <t>Handling</t>
+  </si>
+  <si>
+    <t>Testfall</t>
+  </si>
+  <si>
+    <t>Öppna sidan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skapa en användare </t>
+  </si>
+  <si>
+    <t>Logga in</t>
+  </si>
+  <si>
+    <t>Logga ut</t>
+  </si>
+  <si>
+    <t>Genomför ett köp</t>
+  </si>
+  <si>
+    <t>Placera en order</t>
+  </si>
+  <si>
+    <t>Lämna en recension</t>
+  </si>
+  <si>
+    <t>Titta på produkterna</t>
+  </si>
+  <si>
+    <t>Gå till http://90.224.160.35/</t>
+  </si>
+  <si>
+    <t>Hemsidan visas</t>
+  </si>
+  <si>
+    <t>Välj en av kategorierna och välj en av tre produkter.</t>
+  </si>
+  <si>
+    <t>Vald produkt visas</t>
+  </si>
+  <si>
+    <t>Välj "Användarsida" och fyll i formuläret.</t>
+  </si>
+  <si>
+    <t>Användaren skapas</t>
+  </si>
+  <si>
+    <t>Inloggningen sker</t>
+  </si>
+  <si>
+    <t>Utloggningen sker</t>
+  </si>
+  <si>
+    <t>Produkten läggs till</t>
+  </si>
+  <si>
+    <t>Gå till kundvagn och tryck på knappen "Slutför köp"</t>
+  </si>
+  <si>
+    <t>Välj en produkt och tryck på knappen "Köp".</t>
+  </si>
+  <si>
+    <t>Välj "Användarsida" och tryck "Logga ut".</t>
+  </si>
+  <si>
+    <t>Välj "Användarsida" och ange dina uppgifter och tryck "Logga in".</t>
+  </si>
+  <si>
+    <t>Tryck på knappen "Lämna en recension" och fyll i formuläret.</t>
+  </si>
+  <si>
+    <t>Recensionen visas</t>
+  </si>
+  <si>
+    <t>Hemsidan skall visas i webläsaren.</t>
+  </si>
+  <si>
+    <t>Den valda produkten skall visas.</t>
+  </si>
+  <si>
+    <t>En användare skall skapas.</t>
+  </si>
+  <si>
+    <t>Du bör loggas ut och returnera till hemvyn.</t>
+  </si>
+  <si>
+    <t>Du bör se din användarsida med ordrar.</t>
+  </si>
+  <si>
+    <t>Produkten skall hamna i din kundvagn.</t>
+  </si>
+  <si>
+    <t>En order skall skapas och kundvagnen skall tömmas.</t>
+  </si>
+  <si>
+    <t>Din recension skall visas under produkten.</t>
+  </si>
+  <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>Ej klar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,15 +183,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,8 +222,19 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -173,38 +243,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -213,75 +261,152 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="20 % - Dekorfärg1" xfId="4" builtinId="30"/>
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
     <cellStyle name="Dålig" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -594,144 +719,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531C8A42-8ABD-40A0-B3FE-7789C8D61459}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
-    <col min="3" max="3" width="91.42578125" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="13">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F7" s="8"/>
+      <c r="G7" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12" t="s">
-        <v>15</v>
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="7" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finns nu testfall för båda användarrollerna
</commit_message>
<xml_diff>
--- a/Administrativa Filer/TestCases.xlsx
+++ b/Administrativa Filer/TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E768C9A-27FA-45C7-AE1F-98AC707657FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEFD8DD-65F6-4549-9D92-8F9C4D7C4D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DFD00660-DC2C-47B0-B7C6-F54E6FD6251E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DFD00660-DC2C-47B0-B7C6-F54E6FD6251E}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -151,6 +151,45 @@
   </si>
   <si>
     <t>Back end klar</t>
+  </si>
+  <si>
+    <t>Användare</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Logga in som admin</t>
+  </si>
+  <si>
+    <t>Adminfunktioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHPmyAdmin </t>
+  </si>
+  <si>
+    <t>Välj "Användarsida" och ange adminuppgifter och tryck "Logga in"</t>
+  </si>
+  <si>
+    <t>Välj "Användarsida" och fyll i ett formulär och tryck på dens knapp</t>
+  </si>
+  <si>
+    <t>Välj "Användarsida" och tryck på knappen märkt "PHPmyAdmin"</t>
+  </si>
+  <si>
+    <t>Du bör se adminsidan</t>
+  </si>
+  <si>
+    <t>Knappen skall utföra det önskade kommandot</t>
+  </si>
+  <si>
+    <t>Du skall omdirigeras till 90.224.160.35/phpmyadmin</t>
+  </si>
+  <si>
+    <t>PHPmyAdmin nås</t>
+  </si>
+  <si>
+    <t>Kommandot utförs</t>
   </si>
 </sst>
 </file>
@@ -369,7 +408,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -383,6 +422,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20 % - Dekorfärg1" xfId="3" builtinId="30"/>
@@ -700,199 +742,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{531C8A42-8ABD-40A0-B3FE-7789C8D61459}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="58.28515625" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" customWidth="1"/>
     <col min="4" max="4" width="46.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="s">
         <v>39</v>
       </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>12</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>